<commit_message>
Add initial project files and configurations for processing
</commit_message>
<xml_diff>
--- a/SCI 1402 Time Keeping.xlsx
+++ b/SCI 1402 Time Keeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c03774c2d788f493/MyDocs/Study/TELUQ/Session 8 - Hiver 2025/SCI 1402/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC104877F95F48285BDE58E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{272C40F5-65D4-4B16-B3FA-86876766B2FB}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="11_F25DC773A252ABDACC104877F95F48285BDE58E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{893CDBBB-470F-41D5-A9B9-6369A85DAFAD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Finalize and submit TN1</t>
+  </si>
+  <si>
+    <t>Target (h)</t>
+  </si>
+  <si>
+    <t>On Target?</t>
+  </si>
+  <si>
+    <t>Exploration on NLP and sentiment analysis</t>
   </si>
 </sst>
 </file>
@@ -99,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,10 +134,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,34 +427,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.109375" customWidth="1"/>
     <col min="2" max="2" width="67.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45698</v>
       </c>
@@ -444,12 +472,16 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" s="3" t="str">
+        <f>IF(E2&lt;&gt;"", D2-E2, "_")</f>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45702</v>
       </c>
@@ -459,12 +491,16 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="str">
+        <f t="shared" ref="F3:F13" si="0">IF(E3&lt;&gt;"", D3-E3, "_")</f>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45706</v>
       </c>
@@ -474,12 +510,19 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>7</v>
@@ -487,12 +530,16 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>8</v>
@@ -500,12 +547,16 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45710</v>
       </c>
@@ -515,12 +566,16 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>10</v>
@@ -528,12 +583,16 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45714</v>
       </c>
@@ -543,12 +602,19 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>12</v>
@@ -556,12 +622,16 @@
       <c r="C10">
         <v>0.5</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>14.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45716</v>
       </c>
@@ -571,12 +641,16 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>16.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>14</v>
@@ -584,12 +658,16 @@
       <c r="C12">
         <v>4</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>20.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45717</v>
       </c>
@@ -599,12 +677,44 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>22.5</v>
       </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>23.5</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="10"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update .gitignore to exclude additional dataset files and update xlsx project books
</commit_message>
<xml_diff>
--- a/SCI 1402 Time Keeping.xlsx
+++ b/SCI 1402 Time Keeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c03774c2d788f493/MyDocs/Study/TELUQ/Session 8 - Hiver 2025/SCI 1402/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="11_F25DC773A252ABDACC104877F95F48285BDE58E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{893CDBBB-470F-41D5-A9B9-6369A85DAFAD}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC104877F95F48285BDE58E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{670B3059-BD31-44EB-8D55-1914760393FA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Exploration on NLP and sentiment analysis</t>
+  </si>
+  <si>
+    <t>Processing datasets</t>
+  </si>
+  <si>
+    <t>Merging and cleaning the combined dataset</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,6 +705,132 @@
       <c r="D14">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
         <v>23.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45718</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45718</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
+        <v>37.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update .gitignore to exclude additional cleaned data files and Excel spreadsheets
</commit_message>
<xml_diff>
--- a/SCI 1402 Time Keeping.xlsx
+++ b/SCI 1402 Time Keeping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c03774c2d788f493/MyDocs/Study/TELUQ/Session 8 - Hiver 2025/SCI 1402/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC104877F95F48285BDE58E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{670B3059-BD31-44EB-8D55-1914760393FA}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC104877F95F48285BDE58E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E200E40E-9EF5-430E-9B1D-0E4140C0C79A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2340" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>Merging and cleaning the combined dataset</t>
+  </si>
+  <si>
+    <t>Finalize data fgathering and cleaning</t>
+  </si>
+  <si>
+    <t>Experiment with first analyses and GUI frameworks</t>
+  </si>
+  <si>
+    <t>Fix issues stemming from lost datatypes in CSVs and incorrect handling of Nas</t>
   </si>
 </sst>
 </file>
@@ -114,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +133,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -149,6 +164,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +453,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +519,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F13" si="0">IF(E3&lt;&gt;"", D3-E3, "_")</f>
+        <f t="shared" ref="F3:F32" si="0">IF(E3&lt;&gt;"", D3-E3, "_")</f>
         <v>_</v>
       </c>
     </row>
@@ -662,11 +679,11 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>20.5</v>
+        <v>21.5</v>
       </c>
       <c r="F12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -674,10 +691,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>45717</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C13">
@@ -685,14 +702,14 @@
       </c>
       <c r="D13">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="E13">
         <v>20</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -704,7 +721,11 @@
       </c>
       <c r="D14">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>23.5</v>
+        <v>24.5</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -715,11 +736,15 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>29.5</v>
+        <v>31.5</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -734,103 +759,201 @@
       </c>
       <c r="D16">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+        <v>39.5</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45721</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
       <c r="D17">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+        <v>41.5</v>
+      </c>
+      <c r="E17">
+        <v>25</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45721</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
       <c r="D18">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+        <v>45.5</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45722</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
       <c r="D19">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D20">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D21">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D22">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D23">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D24">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D26">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D27">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D29">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D30">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D31">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+        <v>48.5</v>
+      </c>
+      <c r="F31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D32">
         <f>SUM(INDEX(C:C,1):INDEX(C:C,ROW()))</f>
-        <v>37.5</v>
+        <v>48.5</v>
+      </c>
+      <c r="F32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
       </c>
     </row>
   </sheetData>

</xml_diff>